<commit_message>
updated chrome ext to include sheet name
</commit_message>
<xml_diff>
--- a/autofill-Chrome/public/Input Script Test 1 June.xlsx
+++ b/autofill-Chrome/public/Input Script Test 1 June.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\prog\autofill\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\prog\autoFill\autofill-Chrome\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{526565C0-5D7C-48B6-80BC-AB0FB24A4A18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B898493-427F-4951-9C3E-90AD02CCAE6C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{22BE58B2-21D0-48B1-85D8-3FEDECB84F64}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{22BE58B2-21D0-48B1-85D8-3FEDECB84F64}"/>
   </bookViews>
   <sheets>
     <sheet name="TEST" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="239" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="240" uniqueCount="65">
   <si>
     <t xml:space="preserve">SARBYN
 </t>
@@ -235,6 +236,9 @@
   </si>
   <si>
     <t>end</t>
+  </si>
+  <si>
+    <t>this is a test sheet</t>
   </si>
 </sst>
 </file>
@@ -660,7 +664,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7C04B7B-859C-40D8-AF26-0DBBB2FF4E7D}">
   <dimension ref="A1:M29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection pane="topRight" activeCell="F14" sqref="F14"/>
     </sheetView>
@@ -1682,4 +1686,22 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{477DE714-1D84-4DB3-8CB3-FAD0C1C40D7B}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>